<commit_message>
word combinations | 1
</commit_message>
<xml_diff>
--- a/all_words.xlsx
+++ b/all_words.xlsx
@@ -458,12 +458,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>leipä</t>
+          <t>harrastaa</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>bread</t>
+          <t>to have (as) a hobby</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -471,19 +471,19 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>verb</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>lompakko</t>
+          <t>kuuma</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>wallet</t>
+          <t>hot</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -491,55 +491,55 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>adjective</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>kaikki</t>
+          <t>kiinni</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>all (determiner)</t>
+          <t>closed</t>
         </is>
       </c>
       <c r="C4" t="n">
         <v>-1</v>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>adjective</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>uikkarit</t>
+          <t>ei mitään</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>swimwear</t>
+          <t>nothing (special)</t>
         </is>
       </c>
       <c r="C5" t="n">
         <v>-1</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>noun</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>keitto</t>
+          <t>kampa</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>soup</t>
+          <t>comb</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -554,72 +554,68 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>harrastaa</t>
+          <t>koti</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>to have (as) a hobby</t>
+          <t>home</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>verb</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>koti</t>
+          <t>kaikki</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>all (determiner)</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>noun</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>huono</t>
+          <t>lompakko</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>bad</t>
+          <t>wallet</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>adjective</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>saari</t>
+          <t>huono</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>island</t>
+          <t>bad</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -627,19 +623,19 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>adjective</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>väärä</t>
+          <t>keitto</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>wrong (adjective)</t>
+          <t>soup</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -647,19 +643,19 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>adjective</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>kuuma</t>
+          <t>leipä</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>hot</t>
+          <t>bread</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -667,19 +663,19 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>adjective</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>taulu</t>
+          <t>uikkarit</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>picture (anything to be put on a wall)</t>
+          <t>swimwear</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -694,12 +690,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>onnellinen</t>
+          <t>väärä</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>wrong (adjective)</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -714,12 +710,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>kenkä</t>
+          <t>seisoa</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>shoe</t>
+          <t>to stand</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -727,19 +723,19 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>verb</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>seisoa</t>
+          <t>ahma</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>to stand</t>
+          <t>wolwerine</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -747,19 +743,19 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>verb</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ahma</t>
+          <t>ystävä</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>wolwerine</t>
+          <t>friend</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -774,12 +770,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>hiki</t>
+          <t>toivoa</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>sweat (body fluid)</t>
+          <t>to hope</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -787,39 +783,35 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>verb</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>kello</t>
+          <t>yksitoista</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>clock</t>
+          <t>eleven</t>
         </is>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>noun</t>
-        </is>
-      </c>
+      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>tyttö</t>
+          <t>sana</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>girl</t>
+          <t>word</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -834,12 +826,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>montako</t>
+          <t>pulassa</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>many (partitive, question)</t>
+          <t>in trouble</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -850,28 +842,32 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>te</t>
+          <t>haista</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>you (plural)</t>
+          <t>to smell (badly)</t>
         </is>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
-      <c r="D22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>verb</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>tori</t>
+          <t>takki</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>market square</t>
+          <t>coat, jacket</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -886,12 +882,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>silta</t>
+          <t>pörröinen</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>bridge</t>
+          <t>fluffy</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -899,19 +895,19 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>adjective</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>halpa</t>
+          <t>grillata</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>cheap</t>
+          <t>to grill</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -919,19 +915,19 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>adjective</t>
+          <t>verb</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>kylmä</t>
+          <t>hiljainen</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>cold</t>
+          <t>quiet (adjective)</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -946,12 +942,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>joki</t>
+          <t>vakava</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>serious</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -959,19 +955,19 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>adjective</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>hauska</t>
+          <t>piilo</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>funny</t>
+          <t>hiding place</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -979,35 +975,39 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>adjective</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>valmis</t>
+          <t>lusikka</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ready</t>
+          <t>spoon</t>
         </is>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
-      <c r="D29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>noun</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>oranssi</t>
+          <t>hotelli</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>orange (color)</t>
+          <t>hotel</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1015,39 +1015,35 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>adjective</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>kahvi</t>
+          <t>minkävärinen</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>coffee</t>
+          <t>what color</t>
         </is>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>noun</t>
-        </is>
-      </c>
+      <c r="D31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>ystävä</t>
+          <t>suositella</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>friend</t>
+          <t>to recommend</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1055,19 +1051,19 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>verb</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>kuu</t>
+          <t>tehdä</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>moon</t>
+          <t>to do, to make</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1075,19 +1071,19 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>verb</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>toivoa</t>
+          <t>ajatella</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>to hope</t>
+          <t>to think (involunteraly)</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1102,16 +1098,16 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>eläin</t>
+          <t>timantti</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>animal</t>
+          <t>diamond</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1122,92 +1118,88 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>pohjoinen</t>
+          <t>yhtään</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>northern</t>
+          <t>any (at all)</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>adjective</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>yksitoista</t>
+          <t>kotona</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>eleven</t>
+          <t>at home</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>prinsessa</t>
+          <t>uusi</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>princess</t>
+          <t>new</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>adjective</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>rahka</t>
+          <t>auki</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>quark</t>
+          <t>open</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>adjective</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>timantti</t>
+          <t>aika</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>diamond</t>
+          <t>time</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1218,108 +1210,112 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>ruskea</t>
+          <t>kanadalainen</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>brown</t>
+          <t>Canadian person</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>adjective</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>älykäs</t>
+          <t>kuu</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>intelligent</t>
+          <t>moon</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>adjective</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>sana</t>
+          <t>koti ikävä</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>home sickness</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>noun</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>enemmän</t>
+          <t>oopperatalo</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>more (not enough)</t>
+          <t>opera house</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>noun</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>uudelleen</t>
+          <t>nätti</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>again (periodically)</t>
+          <t>pretty (adjective)</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
-      </c>
-      <c r="D45" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>adjective</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>krokotiili</t>
+          <t>käärme</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>crocodile</t>
+          <t>snake</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1330,212 +1326,212 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>yhtään</t>
+          <t>jee</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>any (at all)</t>
+          <t>yay</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Tyyne</t>
+          <t>hiki</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Tyyne</t>
+          <t>sweat (body fluid)</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
-      </c>
-      <c r="D48" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>noun</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>hirvi</t>
+          <t>halpa</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>moose</t>
+          <t>cheap</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>adjective</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>lause</t>
+          <t>miten</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>sentence</t>
+          <t>how (+ usein)</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>noun</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>aika</t>
+          <t>montako</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>time</t>
+          <t>many (partitive, question)</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>noun</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>käärme</t>
+          <t>lisää</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>snake</t>
+          <t>more (of something)</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>noun</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>pulassa</t>
+          <t>Tyyne</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>in trouble</t>
+          <t>Tyyne</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>ja</t>
+          <t>pohjoinen</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>and</t>
+          <t>northern</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
-      </c>
-      <c r="D54" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>adjective</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>haista</t>
+          <t>rakennus</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>to smell (badly)</t>
+          <t>building</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>verb</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>nopeasti</t>
+          <t>tori</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>quickly (adverb)</t>
+          <t>market square</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
-      </c>
-      <c r="D56" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>noun</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>miau</t>
+          <t>anteeksi</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>meow (cat sound)</t>
+          <t>excuse me</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>ketsuppi</t>
+          <t>unkari</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>ketchup</t>
+          <t>Hungarian language</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1546,48 +1542,52 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>miten</t>
+          <t>olla ostoksilla</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>how (+ usein)</t>
+          <t>to be shopping</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>koti ikävä</t>
+          <t>salmiakki</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>home sickness</t>
+          <t>salmiakki</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
-      </c>
-      <c r="D60" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>noun</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>takki</t>
+          <t>riisi</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>coat, jacket</t>
+          <t>rice</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -1598,92 +1598,92 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>pörröinen</t>
+          <t>kulta</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>fluffy</t>
+          <t>darling</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>adjective</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>olla ostoksilla</t>
+          <t>älykäs</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>to be shopping</t>
+          <t>intelligent</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D63" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>adjective</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>salmiakki</t>
+          <t>ruskea</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>salmiakki</t>
+          <t>brown</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>adjective</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>grillata</t>
+          <t>kello</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>to grill</t>
+          <t>clock</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>verb</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>lamppu</t>
+          <t>kaupunki</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>lamp</t>
+          <t>city</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -1694,52 +1694,56 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>kotona</t>
+          <t>kahvi</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>at home</t>
+          <t>coffee</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
-      </c>
-      <c r="D67" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>noun</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>nätti</t>
+          <t>joki</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>pretty (adjective)</t>
+          <t>river</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>adjective</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>turisti</t>
+          <t>helmi</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>tourist</t>
+          <t>pearl</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -1750,176 +1754,168 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>kiinni</t>
+          <t>Lontoo</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>closed</t>
+          <t>London</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>adjective</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>hiljainen</t>
+          <t>kenkä</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>quiet (adjective)</t>
+          <t>shoe</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>adjective</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>sotkuinen</t>
+          <t>tyttö</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>messy</t>
+          <t>girl</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>adjective</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>vakava</t>
+          <t>saari</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>serious</t>
+          <t>island</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>adjective</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>uusi</t>
+          <t>neljä</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>four</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>adjective</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>auki</t>
+          <t>turisti</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>open</t>
+          <t>tourist</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>adjective</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>piilo</t>
+          <t>sotkuinen</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>hiding place</t>
+          <t>messy</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>adjective</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Lontoo</t>
+          <t>mikä</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>London</t>
+          <t>what (object)</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>noun</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>oopperatalo</t>
+          <t>lause</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>opera house</t>
+          <t>sentence</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -1930,16 +1926,16 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>unkari</t>
+          <t>Berliini</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Hungarian language</t>
+          <t>Berlin</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -1950,16 +1946,16 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>lusikka</t>
+          <t>prinsessa</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>spoon</t>
+          <t>princess</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -1970,36 +1966,36 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>hotelli</t>
+          <t>oranssi</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>hotel</t>
+          <t>orange (color)</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>adjective</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>kanadalainen</t>
+          <t>hirvi</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Canadian person</t>
+          <t>moose</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -2010,16 +2006,16 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Berliini</t>
+          <t>ketsuppi</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Berlin</t>
+          <t>ketchup</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -2030,76 +2026,68 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>rakennus</t>
+          <t>nyt</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>building</t>
+          <t>now</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>noun</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>velho</t>
+          <t>onnellinen</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>wizard</t>
+          <t>happy</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>adjective</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>pasta</t>
+          <t>te</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>pasta</t>
+          <t>you (plural)</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>noun</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>kivi</t>
+          <t>rahka</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>stone, rock</t>
+          <t>quark</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -2110,96 +2098,80 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>tabletti</t>
+          <t>valmis</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>tablet</t>
+          <t>ready</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>noun</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>kampa</t>
+          <t>vaikka</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>comb</t>
+          <t>although</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>noun</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>ruoka</t>
+          <t>uudelleen</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>food</t>
+          <t>again (periodically)</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>noun</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>helmi</t>
+          <t>enemmän</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>pearl</t>
+          <t>more (not enough)</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>noun</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>lumi</t>
+          <t>velho</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>snow</t>
+          <t>wizard</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -2210,36 +2182,36 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>kaupunki</t>
+          <t>kylmä</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>city</t>
+          <t>cold</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>adjective</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>riisi</t>
+          <t>taulu</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>rice</t>
+          <t>picture (anything to be put on a wall)</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -2250,238 +2222,266 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>nyt</t>
+          <t>lumi</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>now</t>
+          <t>snow</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>0</v>
-      </c>
-      <c r="D95" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>noun</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>vaikka</t>
+          <t>ja</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>although</t>
+          <t>and</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>minkävärinen</t>
+          <t>hauska</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>what color</t>
+          <t>funny</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>0</v>
-      </c>
-      <c r="D97" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>adjective</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>kulta</t>
+          <t>ruoka</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>darling</t>
+          <t>food</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0</v>
-      </c>
-      <c r="D98" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>noun</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>suositella</t>
+          <t>nopeasti</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>to recommend</t>
+          <t>quickly (adverb)</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>0</v>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>verb</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>tehdä</t>
+          <t>kivi</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>to do, to make</t>
+          <t>stone, rock</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>verb</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>neljä</t>
+          <t>mur</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>four</t>
+          <t>growl (bear sound)</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>jee</t>
+          <t>lamppu</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>yay</t>
+          <t>lamp</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>0</v>
-      </c>
-      <c r="D102" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>noun</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>mikä</t>
+          <t>silta</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>what (object)</t>
+          <t>bridge</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
-      </c>
-      <c r="D103" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>noun</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>ei mitään</t>
+          <t>eläin</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>nothing (special)</t>
+          <t>animal</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>0</v>
-      </c>
-      <c r="D104" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>noun</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>ajatella</t>
+          <t>pasta</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>to think (involunteraly)</t>
+          <t>pasta</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>verb</t>
+          <t>noun</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>mur</t>
+          <t>krokotiili</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>growl (bear sound)</t>
+          <t>crocodile</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>0</v>
-      </c>
-      <c r="D106" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>noun</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>anteeksi</t>
+          <t>miau</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>excuse me</t>
+          <t>meow (cat sound)</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>lisää</t>
+          <t>tabletti</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>more (of something)</t>
+          <t>tablet</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>0</v>
-      </c>
-      <c r="D108" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>noun</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">

</xml_diff>

<commit_message>
word combinations | combinations are ready to be tested
</commit_message>
<xml_diff>
--- a/all_words.xlsx
+++ b/all_words.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>American person</t>
+          <t>American (adjective)</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -491,19 +491,19 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>noun</t>
+          <t>adjective</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>amerikkalainen</t>
+          <t>seisoa</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>American (adjective)</t>
+          <t>to stand</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -511,19 +511,19 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>adjective</t>
+          <t>verb</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>seisoa</t>
+          <t>toivoa</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>to stand</t>
+          <t>to hope</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -538,12 +538,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>toivoa</t>
+          <t>haista</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>to hope</t>
+          <t>to smell (badly)</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -558,12 +558,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>haista</t>
+          <t>grillata</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>to smell (badly)</t>
+          <t>to grill</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -578,12 +578,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>grillata</t>
+          <t>suositella</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>to grill</t>
+          <t>to recommend</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -598,12 +598,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>suositella</t>
+          <t>tehdä</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>to recommend</t>
+          <t>to do, to make</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -618,12 +618,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>tehdä</t>
+          <t>ajatella</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>to do, to make</t>
+          <t>to think (involunteraly)</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -638,32 +638,28 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ajatella</t>
+          <t>lisää</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>to think (involunteraly)</t>
+          <t>more (of something)</t>
         </is>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>verb</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>lisää</t>
+          <t>yhtään</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>more (of something)</t>
+          <t>any (at all)</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -674,18 +670,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>yhtään</t>
+          <t>amerikkalainen</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>any (at all)</t>
+          <t>American person</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>noun</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">

</xml_diff>